<commit_message>
Adding to my Evaluation.
</commit_message>
<xml_diff>
--- a/src/Pred_actual.xlsx
+++ b/src/Pred_actual.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinckley/Desktop/Comp/COMP Github repo/Predicting-NBA-contracts/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D43311-8A85-F844-9EBA-636FC03E9543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79A9A95-D798-2548-9D79-F13C47BD82B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="303">
   <si>
     <t>Actual Ave Salary</t>
   </si>
@@ -926,13 +939,16 @@
   </si>
   <si>
     <t>Derrick Walton Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -954,6 +970,14 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -970,7 +994,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -993,18 +1017,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1308,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I22" sqref="I21:I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1320,9 +1357,10 @@
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1332,11 +1370,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E1" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50203930</v>
       </c>
@@ -1349,8 +1390,12 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f>A2-B2</f>
+        <v>40298193.456299737</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>43031940</v>
       </c>
@@ -1363,8 +1408,12 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="0">A3-B3</f>
+        <v>22835891.183525089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>34320000</v>
       </c>
@@ -1377,8 +1426,12 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>31605305.555900544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>33232282</v>
       </c>
@@ -1391,8 +1444,12 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5871433.8810100816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>26000000</v>
       </c>
@@ -1405,8 +1462,12 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>8933837.9532990307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>25000000</v>
       </c>
@@ -1419,8 +1480,12 @@
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>9087819.5520882998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>17737500</v>
       </c>
@@ -1433,8 +1498,12 @@
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>15254266.193665504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>17500000</v>
       </c>
@@ -1447,8 +1516,12 @@
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>8180001.854722973</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16500000</v>
       </c>
@@ -1461,8 +1534,12 @@
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>9531703.0474445038</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>15000000</v>
       </c>
@@ -1475,8 +1552,12 @@
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-1497918.8463349305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>14500000</v>
       </c>
@@ -1489,8 +1570,12 @@
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2552751.2926005591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12500000</v>
       </c>
@@ -1503,8 +1588,12 @@
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>9361047.0030134767</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12144552</v>
       </c>
@@ -1517,8 +1606,12 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-388435.10582266934</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11750000</v>
       </c>
@@ -1531,8 +1624,12 @@
       <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1223534.6617621109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>11277084</v>
       </c>
@@ -1545,8 +1642,12 @@
       <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2844616.4196328819</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11014500</v>
       </c>
@@ -1559,8 +1660,12 @@
       <c r="D17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2105639.0090671405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>10300000</v>
       </c>
@@ -1573,8 +1678,12 @@
       <c r="D18" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>-4925844.6606595702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9709025</v>
       </c>
@@ -1587,8 +1696,12 @@
       <c r="D19" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>-4227250.2769270204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9100000</v>
       </c>
@@ -1601,8 +1714,12 @@
       <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1161421.0282558221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9000000</v>
       </c>
@@ -1615,8 +1732,12 @@
       <c r="D21" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>-2829156.1205133498</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8715000</v>
       </c>
@@ -1629,8 +1750,12 @@
       <c r="D22" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>-2440941.7318041194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8625000</v>
       </c>
@@ -1643,8 +1768,12 @@
       <c r="D23" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>4209599.0178238181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8000000</v>
       </c>
@@ -1657,8 +1786,12 @@
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>-3129698.9347183201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8000000</v>
       </c>
@@ -1671,8 +1804,12 @@
       <c r="D25" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>4266561.0055616442</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7840000</v>
       </c>
@@ -1685,8 +1822,12 @@
       <c r="D26" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>-5991304.0885838307</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7500000</v>
       </c>
@@ -1699,8 +1840,12 @@
       <c r="D27" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>3224560.6022814075</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>6876811</v>
       </c>
@@ -1713,8 +1858,12 @@
       <c r="D28" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>-4405970.9177188091</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6802950</v>
       </c>
@@ -1727,8 +1876,12 @@
       <c r="D29" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>-646114.16263553686</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>6640975</v>
       </c>
@@ -1741,8 +1894,12 @@
       <c r="D30" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>3239944.7686484181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>6640975</v>
       </c>
@@ -1755,8 +1912,12 @@
       <c r="D31" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>-8510515.0689164791</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>6640975</v>
       </c>
@@ -1769,8 +1930,12 @@
       <c r="D32" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>4603868.7441240679</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6640975</v>
       </c>
@@ -1783,8 +1948,12 @@
       <c r="D33" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>-1773997.3823099211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>6479000</v>
       </c>
@@ -1797,8 +1966,12 @@
       <c r="D34" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>-4943743.5021764003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6479000</v>
       </c>
@@ -1811,8 +1984,12 @@
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>3847407.7466722359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6150000</v>
       </c>
@@ -1825,8 +2002,12 @@
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>-560242.78121181671</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6146342</v>
       </c>
@@ -1839,8 +2020,12 @@
       <c r="D37" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>-10023541.88276246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5734280</v>
       </c>
@@ -1853,8 +2038,12 @@
       <c r="D38" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>-4573495.3625229094</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5043773</v>
       </c>
@@ -1867,8 +2056,12 @@
       <c r="D39" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>-53589.969914007001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4612500</v>
       </c>
@@ -1881,8 +2074,12 @@
       <c r="D40" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>-983125.37805124745</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4512000</v>
       </c>
@@ -1895,8 +2092,12 @@
       <c r="D41" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>1792931.7563862428</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4207625</v>
       </c>
@@ -1909,8 +2110,12 @@
       <c r="D42" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>-1230543.5955364583</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3666667</v>
       </c>
@@ -1923,8 +2128,12 @@
       <c r="D43" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>-5137573.5390825905</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3500000</v>
       </c>
@@ -1937,8 +2146,12 @@
       <c r="D44" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>-1208094.8131413376</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3280000</v>
       </c>
@@ -1951,8 +2164,12 @@
       <c r="D45" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>-1681775.1849707179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3280000</v>
       </c>
@@ -1965,8 +2182,12 @@
       <c r="D46" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>-7272708.1353236903</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3000000</v>
       </c>
@@ -1979,8 +2200,12 @@
       <c r="D47" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>1124373.5896602341</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2905851</v>
       </c>
@@ -1993,8 +2218,12 @@
       <c r="D48" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>-390208.04300838988</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2905851</v>
       </c>
@@ -2007,8 +2236,12 @@
       <c r="D49" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>-962825.04288872378</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2905851</v>
       </c>
@@ -2021,8 +2254,12 @@
       <c r="D50" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>-582655.22163757496</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2905851</v>
       </c>
@@ -2035,8 +2272,12 @@
       <c r="D51" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>1336390.5556612101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2905851</v>
       </c>
@@ -2049,8 +2290,12 @@
       <c r="D52" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>-4132076.0082913693</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2905851</v>
       </c>
@@ -2063,8 +2308,12 @@
       <c r="D53" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>-1954976.059648904</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2905851</v>
       </c>
@@ -2077,8 +2326,12 @@
       <c r="D54" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>370482.3359868289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2905851</v>
       </c>
@@ -2091,8 +2344,12 @@
       <c r="D55" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>-1089665.2288034149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2905851</v>
       </c>
@@ -2105,8 +2362,12 @@
       <c r="D56" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>-1679777.4267409472</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2905851</v>
       </c>
@@ -2119,8 +2380,12 @@
       <c r="D57" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>-15738200.461884379</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2905851</v>
       </c>
@@ -2133,8 +2398,12 @@
       <c r="D58" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>2355135.1060001096</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2900000</v>
       </c>
@@ -2147,8 +2416,12 @@
       <c r="D59" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>1072485.3843175301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2641682</v>
       </c>
@@ -2161,8 +2434,12 @@
       <c r="D60" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>-881814.61775197322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2641682</v>
       </c>
@@ -2175,8 +2452,12 @@
       <c r="D61" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>-90507.6421566559</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2628597</v>
       </c>
@@ -2189,8 +2470,12 @@
       <c r="D62" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>2287472.7461935719</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2628597</v>
       </c>
@@ -2203,8 +2488,12 @@
       <c r="D63" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>-121087.84021385387</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2628597</v>
       </c>
@@ -2217,8 +2506,12 @@
       <c r="D64" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>-772433.23135158187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2611758</v>
       </c>
@@ -2231,8 +2524,12 @@
       <c r="D65" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>347214.16938048601</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2463490</v>
       </c>
@@ -2245,8 +2542,12 @@
       <c r="D66" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>-1650118.8156895051</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2463490</v>
       </c>
@@ -2259,8 +2560,12 @@
       <c r="D67" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <f t="shared" ref="E67:E123" si="1">A67-B67</f>
+        <v>-413035.02612854401</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2442525</v>
       </c>
@@ -2273,8 +2578,12 @@
       <c r="D68" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <f t="shared" si="1"/>
+        <v>-530223.61544313701</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2298385</v>
       </c>
@@ -2287,8 +2596,12 @@
       <c r="D69" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <f t="shared" si="1"/>
+        <v>-1867709.4098611008</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2298385</v>
       </c>
@@ -2301,8 +2614,12 @@
       <c r="D70" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <f t="shared" si="1"/>
+        <v>1305915.3550558444</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2298385</v>
       </c>
@@ -2315,8 +2632,12 @@
       <c r="D71" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <f t="shared" si="1"/>
+        <v>-499411.6348711499</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2298385</v>
       </c>
@@ -2329,8 +2650,12 @@
       <c r="D72" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <f t="shared" si="1"/>
+        <v>-3236007.1848510513</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2273291</v>
       </c>
@@ -2343,8 +2668,12 @@
       <c r="D73" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <f t="shared" si="1"/>
+        <v>-1342055.407552266</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2273291</v>
       </c>
@@ -2357,8 +2686,12 @@
       <c r="D74" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <f t="shared" si="1"/>
+        <v>-2006522.1972328918</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2271775</v>
       </c>
@@ -2371,8 +2704,12 @@
       <c r="D75" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <f t="shared" si="1"/>
+        <v>-1417925.999295359</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2200000</v>
       </c>
@@ -2385,8 +2722,12 @@
       <c r="D76" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <f t="shared" si="1"/>
+        <v>-2241643.7792619793</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2187500</v>
       </c>
@@ -2399,8 +2740,12 @@
       <c r="D77" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <f t="shared" si="1"/>
+        <v>-3513096.566394438</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2169972</v>
       </c>
@@ -2413,8 +2758,12 @@
       <c r="D78" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <f t="shared" si="1"/>
+        <v>-5917316.1552303657</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2133278</v>
       </c>
@@ -2427,8 +2776,12 @@
       <c r="D79" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <f t="shared" si="1"/>
+        <v>-1359602.0211518751</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2133278</v>
       </c>
@@ -2441,8 +2794,12 @@
       <c r="D80" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <f t="shared" si="1"/>
+        <v>-2181525.5933472896</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2133278</v>
       </c>
@@ -2455,8 +2812,12 @@
       <c r="D81" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <f t="shared" si="1"/>
+        <v>-2054685.407432599</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2133278</v>
       </c>
@@ -2469,8 +2830,12 @@
       <c r="D82" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <f t="shared" si="1"/>
+        <v>983351.5725410569</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2133278</v>
       </c>
@@ -2483,8 +2848,12 @@
       <c r="D83" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <f t="shared" si="1"/>
+        <v>-957563.20232922817</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1984359</v>
       </c>
@@ -2497,8 +2866,12 @@
       <c r="D84" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <f t="shared" si="1"/>
+        <v>2040899.7655019192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1984359</v>
       </c>
@@ -2511,8 +2884,12 @@
       <c r="D85" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <f t="shared" si="1"/>
+        <v>-1626613.6080379658</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1968185</v>
       </c>
@@ -2525,8 +2902,12 @@
       <c r="D86" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <f t="shared" si="1"/>
+        <v>-3098561.3733139094</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1968175</v>
       </c>
@@ -2539,8 +2920,12 @@
       <c r="D87" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <f t="shared" si="1"/>
+        <v>-3059207.1776852123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1968175</v>
       </c>
@@ -2553,8 +2938,12 @@
       <c r="D88" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <f t="shared" si="1"/>
+        <v>-2333507.1948043909</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1968175</v>
       </c>
@@ -2567,8 +2956,12 @@
       <c r="D89" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <f t="shared" si="1"/>
+        <v>-3570590.9843653506</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1968175</v>
       </c>
@@ -2581,8 +2974,12 @@
       <c r="D90" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <f t="shared" si="1"/>
+        <v>-1651545.2070665648</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1968175</v>
       </c>
@@ -2595,8 +2992,12 @@
       <c r="D91" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <f t="shared" si="1"/>
+        <v>-2246031.2045183973</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1968175</v>
       </c>
@@ -2609,8 +3010,12 @@
       <c r="D92" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <f t="shared" si="1"/>
+        <v>-1074554.4076719312</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1916664</v>
       </c>
@@ -2623,8 +3028,12 @@
       <c r="D93" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <f t="shared" si="1"/>
+        <v>-1576216.0211518751</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1916664</v>
       </c>
@@ -2637,8 +3046,12 @@
       <c r="D94" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <f t="shared" si="1"/>
+        <v>-4343428.1677318737</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1902133</v>
       </c>
@@ -2651,8 +3064,12 @@
       <c r="D95" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <f t="shared" si="1"/>
+        <v>-3173360.9723425088</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1902133</v>
       </c>
@@ -2665,8 +3082,12 @@
       <c r="D96" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <f t="shared" si="1"/>
+        <v>4577176.728595729</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1902133</v>
       </c>
@@ -2679,8 +3100,12 @@
       <c r="D97" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <f t="shared" si="1"/>
+        <v>-1612616.0187233728</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1902133</v>
       </c>
@@ -2693,8 +3118,12 @@
       <c r="D98" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <f t="shared" si="1"/>
+        <v>-1761325.2022095621</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1902133</v>
       </c>
@@ -2707,8 +3136,12 @@
       <c r="D99" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <f t="shared" si="1"/>
+        <v>-1018130.0212715408</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1902133</v>
       </c>
@@ -2721,8 +3154,12 @@
       <c r="D100" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <f t="shared" si="1"/>
+        <v>118356.3794605271</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1886069</v>
       </c>
@@ -2735,8 +3172,12 @@
       <c r="D101" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <f t="shared" si="1"/>
+        <v>-2507462.9846046837</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1886069</v>
       </c>
@@ -2749,8 +3190,12 @@
       <c r="D102" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <f t="shared" si="1"/>
+        <v>2637693.151782643</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1836090</v>
       </c>
@@ -2763,8 +3208,12 @@
       <c r="D103" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <f t="shared" si="1"/>
+        <v>1201921.1787354946</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1836090</v>
       </c>
@@ -2777,8 +3226,12 @@
       <c r="D104" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <f t="shared" si="1"/>
+        <v>-1783630.2070665648</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1836090</v>
       </c>
@@ -2791,8 +3244,12 @@
       <c r="D105" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <f t="shared" si="1"/>
+        <v>-1818620.6031809631</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1836090</v>
       </c>
@@ -2805,8 +3262,12 @@
       <c r="D106" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <f t="shared" si="1"/>
+        <v>-4493982.9599606683</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1836090</v>
       </c>
@@ -2819,8 +3280,12 @@
       <c r="D107" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <f t="shared" si="1"/>
+        <v>-1311610.5960151232</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1836090</v>
       </c>
@@ -2833,8 +3298,12 @@
       <c r="D108" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <f t="shared" si="1"/>
+        <v>-1853610.999295359</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1836090</v>
       </c>
@@ -2847,8 +3316,12 @@
       <c r="D109" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <f t="shared" si="1"/>
+        <v>1315639.9661072856</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1836090</v>
       </c>
@@ -2861,8 +3334,12 @@
       <c r="D110" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <f t="shared" si="1"/>
+        <v>-1879853.7963811569</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>1836090</v>
       </c>
@@ -2875,8 +3352,12 @@
       <c r="D111" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <f t="shared" si="1"/>
+        <v>-1989198.7842386491</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1836090</v>
       </c>
@@ -2889,8 +3370,12 @@
       <c r="D112" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <f t="shared" si="1"/>
+        <v>-1219760.8062148299</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1836090</v>
       </c>
@@ -2903,8 +3388,12 @@
       <c r="D113" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <f t="shared" si="1"/>
+        <v>-1578061.629894481</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1782931</v>
       </c>
@@ -2917,8 +3406,12 @@
       <c r="D114" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <f t="shared" si="1"/>
+        <v>-2055479.1827815478</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1782931</v>
       </c>
@@ -2931,8 +3424,12 @@
       <c r="D115" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <f t="shared" si="1"/>
+        <v>-2090469.5788959451</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1637966</v>
       </c>
@@ -2945,8 +3442,12 @@
       <c r="D116" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <f t="shared" si="1"/>
+        <v>-1951137.6104664672</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1637966</v>
       </c>
@@ -2959,8 +3460,12 @@
       <c r="D117" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <f t="shared" si="1"/>
+        <v>-2112968.1924955552</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>1637966</v>
       </c>
@@ -2973,8 +3478,12 @@
       <c r="D118" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <f t="shared" si="1"/>
+        <v>-1435380.0042720288</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1637966</v>
       </c>
@@ -2987,8 +3496,12 @@
       <c r="D119" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <f t="shared" si="1"/>
+        <v>-1881156.818237673</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1637966</v>
       </c>
@@ -3001,8 +3514,12 @@
       <c r="D120" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <f t="shared" si="1"/>
+        <v>-1588462.9872725168</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1637966</v>
       </c>
@@ -3015,8 +3532,12 @@
       <c r="D121" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <f t="shared" si="1"/>
+        <v>-2042987.40026676</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>1637966</v>
       </c>
@@ -3029,8 +3550,12 @@
       <c r="D122" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E122">
+        <f t="shared" si="1"/>
+        <v>-2847415.7744049774</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1637966</v>
       </c>
@@ -3043,28 +3568,32 @@
       <c r="D123" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <f t="shared" si="1"/>
+        <v>-819025.00924869906</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D124" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D125" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D126" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D127" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D128" s="3" t="s">
         <v>130</v>
       </c>

</xml_diff>